<commit_message>
QMM017 #3156 , Update template file
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM017.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM017.xlsx
@@ -44508,7 +44508,7 @@
     <col min="11" max="11" width="40.7109375" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.140625" style="1" customWidth="1"/>
     <col min="13" max="15" width="17" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="1.140625" style="1" customWidth="1"/>
     <col min="18" max="18" width="10.7109375" style="1" customWidth="1"/>
     <col min="19" max="16384" width="10.7109375" style="1"/>
@@ -44651,7 +44651,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.2" right="0.2" top="0.66249999999999998" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="54" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,標準"&amp;10日通システム株式会社 &amp;C&amp;"ＭＳ ゴシック,標準"&amp;16計算式の登録 &amp;R&amp;"ＭＳ ゴシック,標準"&amp;10&amp;KFF0000 &amp;K01+000     &amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000          page&amp;P</oddHeader>

</xml_diff>